<commit_message>
run code with 2019
updated do files to include 2019. run code to aggregate to geographies. added new names to crosswalk.
</commit_message>
<xml_diff>
--- a/raw/cvp/deliveries/deliveries 2011-2019.xlsx
+++ b/raw/cvp/deliveries/deliveries 2011-2019.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jeffh\OneDrive\Documents\UCDavis\data-surface-water\raw\cvp\deliveries\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34F98E7-D585-4037-9D62-5EFC4BEA88A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E125A48-0405-45A9-92AD-78199037E6DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="6" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="19392" windowHeight="10392" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="22" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4506" uniqueCount="339">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4506" uniqueCount="336">
   <si>
     <t>Friant-Kern Canal</t>
   </si>
@@ -1484,9 +1484,6 @@
     <t>CROSS VALLEY CANAL</t>
   </si>
   <si>
-    <t>Tranquility Public Utilities District (TPUD) (formerly Hughes, Melvin)</t>
-  </si>
-  <si>
     <t>Mid-Valley WD (no contract)(Kings River)</t>
   </si>
   <si>
@@ -1500,12 +1497,6 @@
   </si>
   <si>
     <t>Los Banos WMA (CDFG) (via CCID &amp; SLCC)</t>
-  </si>
-  <si>
-    <t>Byron Bethany ID (formerly Plainview WD )</t>
-  </si>
-  <si>
-    <t>Panoche WD -</t>
   </si>
   <si>
     <t>Grasslands WD (76.05/Los Banos Creek &amp; CCID)</t>
@@ -1569,7 +1560,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1630,6 +1621,12 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="3" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -27463,13 +27460,13 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
   <dimension ref="A1:Q264"/>
   <sheetViews>
-    <sheetView topLeftCell="A241" workbookViewId="0">
-      <selection activeCell="D254" sqref="D254:D264"/>
+    <sheetView tabSelected="1" topLeftCell="A223" workbookViewId="0">
+      <selection activeCell="A237" sqref="A237"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="11.4" x14ac:dyDescent="0.4"/>
   <cols>
-    <col min="1" max="1" width="55.578125" style="4" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="49.20703125" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="26.15625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="18.68359375" style="4" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="6.68359375" style="4" bestFit="1" customWidth="1"/>
@@ -27582,8 +27579,8 @@
         <v>755</v>
       </c>
     </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A3" s="3" t="s">
+    <row r="3" spans="1:17" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="A3" s="24" t="s">
         <v>236</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -29089,8 +29086,8 @@
         <v>1103</v>
       </c>
     </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A32" s="3" t="s">
+    <row r="32" spans="1:17" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="A32" s="24" t="s">
         <v>236</v>
       </c>
       <c r="B32" s="3" t="s">
@@ -39642,9 +39639,9 @@
         <v>1602</v>
       </c>
     </row>
-    <row r="236" spans="1:17" x14ac:dyDescent="0.4">
-      <c r="A236" s="4" t="s">
-        <v>329</v>
+    <row r="236" spans="1:17" ht="22.8" x14ac:dyDescent="0.4">
+      <c r="A236" s="25" t="s">
+        <v>236</v>
       </c>
       <c r="B236" s="3" t="s">
         <v>82</v>
@@ -39844,7 +39841,7 @@
     </row>
     <row r="240" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A240" s="4" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="B240" s="3" t="s">
         <v>82</v>
@@ -40094,7 +40091,7 @@
     </row>
     <row r="245" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A245" s="4" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="B245" s="3" t="s">
         <v>82</v>
@@ -40244,7 +40241,7 @@
     </row>
     <row r="248" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A248" s="4" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="B248" s="3" t="s">
         <v>82</v>
@@ -40350,7 +40347,7 @@
         <v>82</v>
       </c>
       <c r="C250" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D250" s="4">
         <v>2019</v>
@@ -40403,7 +40400,7 @@
         <v>82</v>
       </c>
       <c r="C251" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D251" s="4">
         <v>2019</v>
@@ -40456,7 +40453,7 @@
         <v>82</v>
       </c>
       <c r="C252" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D252" s="4">
         <v>2019</v>
@@ -40509,7 +40506,7 @@
         <v>82</v>
       </c>
       <c r="C253" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D253" s="4">
         <v>2019</v>
@@ -40562,7 +40559,7 @@
         <v>82</v>
       </c>
       <c r="C254" s="4" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="D254" s="4">
         <v>2019</v>
@@ -40715,7 +40712,7 @@
     </row>
     <row r="257" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A257" s="4" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="B257" s="3" t="s">
         <v>82</v>
@@ -41143,8 +41140,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Q307"/>
   <sheetViews>
-    <sheetView topLeftCell="A289" workbookViewId="0">
-      <selection activeCell="B311" sqref="B311"/>
+    <sheetView topLeftCell="A270" workbookViewId="0">
+      <selection activeCell="A284" sqref="A284"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="11.4" x14ac:dyDescent="0.4"/>
@@ -55313,7 +55310,7 @@
     </row>
     <row r="275" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A275" s="4" t="s">
-        <v>335</v>
+        <v>256</v>
       </c>
       <c r="B275" s="3" t="s">
         <v>92</v>
@@ -55763,7 +55760,7 @@
     </row>
     <row r="284" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A284" s="4" t="s">
-        <v>336</v>
+        <v>102</v>
       </c>
       <c r="B284" s="3" t="s">
         <v>92</v>
@@ -56537,7 +56534,7 @@
     </row>
     <row r="299" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A299" s="4" t="s">
-        <v>337</v>
+        <v>334</v>
       </c>
       <c r="B299" s="3" t="s">
         <v>92</v>
@@ -78277,8 +78274,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0600-000000000000}">
   <dimension ref="A1:Q428"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A225" workbookViewId="0">
-      <selection activeCell="D381" sqref="D381:D428"/>
+    <sheetView topLeftCell="A374" workbookViewId="0">
+      <selection activeCell="A387" sqref="A387"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.15625" defaultRowHeight="11.4" x14ac:dyDescent="0.4"/>
@@ -97836,7 +97833,7 @@
     </row>
     <row r="387" spans="1:17" x14ac:dyDescent="0.4">
       <c r="A387" s="4" t="s">
-        <v>338</v>
+        <v>335</v>
       </c>
       <c r="B387" s="4" t="s">
         <v>276</v>

</xml_diff>